<commit_message>
added debug ability to download excel from service account
</commit_message>
<xml_diff>
--- a/app/src/main/assets/report_rmi.xlsx
+++ b/app/src/main/assets/report_rmi.xlsx
@@ -3,28 +3,54 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Standard Scores Summary" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="template" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Standard Scores Summary" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="template" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName localSheetId="1" name="_Hlk5874819">#REF!</definedName>
   </definedNames>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mg9rGqJIgdD2XT4kfksn5ywlgFDlQ=="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="246">
+  <si>
+    <t>Summary of School Evaluation Scores</t>
+  </si>
+  <si>
+    <t>Summary of Classroom Observation 1 Scores</t>
+  </si>
   <si>
     <t>SCHOOL ACCREDITATION STATUS REPORT – FORM B</t>
   </si>
   <si>
+    <t>Summary of Classroom Observation 2 Scores</t>
+  </si>
+  <si>
     <t>Note this is a preview of the FORM B only. The results are not final and official until verified and signed by the SDOE Director and the NDOE Secretary</t>
   </si>
   <si>
+    <t>School Number</t>
+  </si>
+  <si>
     <t>$schNo</t>
   </si>
   <si>
+    <t>School Name</t>
+  </si>
+  <si>
+    <t>Survey Date</t>
+  </si>
+  <si>
+    <t>Standard 1</t>
+  </si>
+  <si>
     <t>$schName</t>
   </si>
   <si>
@@ -37,25 +63,19 @@
     <t>Summary of School Evaluation/Classroom Observation Scores</t>
   </si>
   <si>
-    <t>Summary of School Evaluation Scores</t>
-  </si>
-  <si>
-    <t>Summary of Classroom Observation 1 Scores</t>
-  </si>
-  <si>
-    <t>Summary of Classroom Observation 2 Scores</t>
-  </si>
-  <si>
-    <t>School Number</t>
-  </si>
-  <si>
-    <t>School Name</t>
-  </si>
-  <si>
-    <t>Survey Date</t>
-  </si>
-  <si>
-    <t>Standard 1</t>
+    <t>Standard 2</t>
+  </si>
+  <si>
+    <t>Standard 3</t>
+  </si>
+  <si>
+    <t>Standard 4</t>
+  </si>
+  <si>
+    <t>Standard 5</t>
+  </si>
+  <si>
+    <t>Standard 6</t>
   </si>
   <si>
     <t>School Evaluation</t>
@@ -64,28 +84,22 @@
     <t>Classroom Observation 1</t>
   </si>
   <si>
-    <t>Standard 2</t>
-  </si>
-  <si>
-    <t>Standard 3</t>
-  </si>
-  <si>
-    <t>Standard 4</t>
-  </si>
-  <si>
-    <t>Standard 5</t>
-  </si>
-  <si>
-    <t>Standard 6</t>
-  </si>
-  <si>
     <t>Classroom Observation 2</t>
   </si>
   <si>
-    <t>AIL100</t>
-  </si>
-  <si>
-    <t>Aerok Elementary School</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
   </si>
   <si>
     <t>Criteria</t>
@@ -749,15 +763,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd.mm.yyyy"/>
-  </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font/>
     <font>
       <sz val="18.0"/>
       <color rgb="FF000000"/>
@@ -769,7 +787,14 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="10.0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -781,23 +806,12 @@
     <font>
       <b/>
       <sz val="8.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font/>
-    <font>
-      <b/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="8.0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8.0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -805,6 +819,11 @@
       <sz val="8.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="7">
@@ -845,7 +864,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border/>
     <border>
       <left/>
@@ -853,11 +872,6 @@
       <bottom/>
     </border>
     <border>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <right/>
       <top/>
       <bottom/>
     </border>
@@ -908,14 +922,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -925,6 +931,14 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
       <top style="thin">
@@ -938,6 +952,18 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+    </border>
+    <border>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
     </border>
     <border>
       <left style="thin">
@@ -986,137 +1012,136 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="8" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="3" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="9" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="12" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="9" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="14" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="8" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1133,6 +1158,200 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+  <a:themeElements>
+    <a:clrScheme name="Sheets">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="FFFFFF"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="0000FF"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Sheets">
+      <a:majorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1152,308 +1371,308 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="7"/>
-      <c r="AG1" s="7"/>
-      <c r="AH1" s="7"/>
-      <c r="AI1" s="7"/>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="7"/>
-      <c r="AL1" s="7"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AO1" s="7"/>
-      <c r="AP1" s="7"/>
-      <c r="AQ1" s="7"/>
-      <c r="AR1" s="7"/>
-      <c r="AS1" s="7"/>
-      <c r="AT1" s="7"/>
-      <c r="AU1" s="7"/>
-      <c r="AV1" s="7"/>
-      <c r="AW1" s="7"/>
-      <c r="AX1" s="7"/>
-      <c r="AY1" s="8"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
+      <c r="AM1" s="3"/>
+      <c r="AN1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO1" s="3"/>
+      <c r="AP1" s="3"/>
+      <c r="AQ1" s="3"/>
+      <c r="AR1" s="3"/>
+      <c r="AS1" s="3"/>
+      <c r="AT1" s="3"/>
+      <c r="AU1" s="3"/>
+      <c r="AV1" s="3"/>
+      <c r="AW1" s="3"/>
+      <c r="AX1" s="3"/>
+      <c r="AY1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15" t="s">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="11" t="s">
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="15" t="s">
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="15" t="s">
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="11"/>
+      <c r="AL2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="13"/>
-      <c r="AG2" s="14"/>
-      <c r="AH2" s="17" t="s">
+      <c r="AM2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="13"/>
-      <c r="AK2" s="14"/>
-      <c r="AL2" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM2" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="AN2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AO2" s="14"/>
-      <c r="AP2" s="15" t="s">
+      <c r="AN2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="11"/>
+      <c r="AT2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="11"/>
+      <c r="AX2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="AQ2" s="13"/>
-      <c r="AR2" s="13"/>
-      <c r="AS2" s="14"/>
-      <c r="AT2" s="17" t="s">
+      <c r="AY2" s="18" t="s">
         <v>17</v>
-      </c>
-      <c r="AU2" s="13"/>
-      <c r="AV2" s="13"/>
-      <c r="AW2" s="14"/>
-      <c r="AX2" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="AY2" s="21" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="25">
-        <v>43473.0</v>
-      </c>
-      <c r="D3" s="26">
-        <v>4.0</v>
-      </c>
-      <c r="E3" s="26">
-        <v>4.0</v>
-      </c>
-      <c r="F3" s="26">
-        <v>4.0</v>
-      </c>
-      <c r="G3" s="26">
-        <v>4.0</v>
-      </c>
-      <c r="H3" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="I3" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="J3" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="K3" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="L3" s="26">
-        <v>4.0</v>
-      </c>
-      <c r="M3" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="N3" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="O3" s="26">
-        <v>4.0</v>
-      </c>
-      <c r="P3" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="Q3" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="R3" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="S3" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="T3" s="26">
-        <v>4.0</v>
-      </c>
-      <c r="U3" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="V3" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="W3" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="X3" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="Y3" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="Z3" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="AA3" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="AB3" s="26">
-        <v>5.0</v>
-      </c>
-      <c r="AC3" s="26">
-        <v>5.0</v>
-      </c>
-      <c r="AD3" s="28">
-        <v>5.0</v>
-      </c>
-      <c r="AE3" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="AF3" s="28">
-        <v>5.0</v>
-      </c>
-      <c r="AG3" s="28">
-        <v>5.0</v>
-      </c>
-      <c r="AH3" s="30">
-        <v>3.0</v>
-      </c>
-      <c r="AI3" s="30">
-        <v>4.0</v>
-      </c>
-      <c r="AJ3" s="30">
-        <v>4.0</v>
-      </c>
-      <c r="AK3" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="AL3" s="28">
-        <v>5.0</v>
-      </c>
-      <c r="AM3" s="26">
-        <v>4.0</v>
-      </c>
-      <c r="AN3" s="26">
-        <v>4.0</v>
-      </c>
-      <c r="AO3" s="26">
-        <v>5.0</v>
-      </c>
-      <c r="AP3" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="AQ3" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="AR3" s="28">
-        <v>5.0</v>
-      </c>
-      <c r="AS3" s="28">
-        <v>5.0</v>
-      </c>
-      <c r="AT3" s="30">
-        <v>3.0</v>
-      </c>
-      <c r="AU3" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="AV3" s="30">
-        <v>3.0</v>
-      </c>
-      <c r="AW3" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="AX3" s="28">
-        <v>5.0</v>
-      </c>
-      <c r="AY3" s="26">
-        <v>5.0</v>
+      <c r="E3" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="U3" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="W3" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC3" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE3" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF3" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG3" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH3" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI3" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ3" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK3" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM3" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="AN3" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO3" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ3" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR3" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="AS3" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="AT3" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="AU3" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="AV3" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="AW3" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="AX3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="AY3" s="30" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
@@ -2436,23 +2655,24 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="AN1:AY1"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="AT2:AW2"/>
+    <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AB1:AM1"/>
     <mergeCell ref="D1:AA1"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="P2:S2"/>
+    <mergeCell ref="X2:AA2"/>
     <mergeCell ref="T2:W2"/>
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AT2:AW2"/>
-    <mergeCell ref="AP2:AS2"/>
-    <mergeCell ref="AN1:AY1"/>
-    <mergeCell ref="AD2:AG2"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2475,279 +2695,279 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
+      <c r="A2" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5"/>
+      <c r="A5" s="9"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7"/>
-      <c r="AE6" s="7"/>
-      <c r="AF6" s="7"/>
-      <c r="AG6" s="7"/>
-      <c r="AH6" s="7"/>
-      <c r="AI6" s="7"/>
-      <c r="AJ6" s="7"/>
-      <c r="AK6" s="7"/>
-      <c r="AL6" s="7"/>
-      <c r="AM6" s="7"/>
-      <c r="AN6" s="7"/>
-      <c r="AO6" s="7"/>
-      <c r="AP6" s="7"/>
-      <c r="AQ6" s="7"/>
-      <c r="AR6" s="7"/>
-      <c r="AS6" s="7"/>
-      <c r="AT6" s="7"/>
-      <c r="AU6" s="7"/>
-      <c r="AV6" s="7"/>
-      <c r="AW6" s="8"/>
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+      <c r="AU6" s="3"/>
+      <c r="AV6" s="3"/>
+      <c r="AW6" s="3"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="8"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
       <c r="Z7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="7"/>
-      <c r="AD7" s="7"/>
-      <c r="AE7" s="7"/>
-      <c r="AF7" s="7"/>
-      <c r="AG7" s="7"/>
-      <c r="AH7" s="7"/>
-      <c r="AI7" s="7"/>
-      <c r="AJ7" s="7"/>
-      <c r="AK7" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
       <c r="AL7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="AM7" s="7"/>
-      <c r="AN7" s="7"/>
-      <c r="AO7" s="7"/>
-      <c r="AP7" s="7"/>
-      <c r="AQ7" s="7"/>
-      <c r="AR7" s="7"/>
-      <c r="AS7" s="7"/>
-      <c r="AT7" s="7"/>
-      <c r="AU7" s="7"/>
-      <c r="AV7" s="7"/>
-      <c r="AW7" s="8"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+      <c r="AU7" s="3"/>
+      <c r="AV7" s="3"/>
+      <c r="AW7" s="3"/>
     </row>
     <row r="8" ht="15.0" customHeight="1">
-      <c r="B8" s="18" t="s">
-        <v>13</v>
+      <c r="B8" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23" t="s">
-        <v>16</v>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22" t="s">
+        <v>14</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="18" t="s">
-        <v>17</v>
+      <c r="I8" s="21"/>
+      <c r="J8" s="19" t="s">
+        <v>15</v>
       </c>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="23" t="s">
-        <v>18</v>
+      <c r="M8" s="21"/>
+      <c r="N8" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="O8" s="20"/>
       <c r="P8" s="20"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="18" t="s">
-        <v>19</v>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="S8" s="20"/>
       <c r="T8" s="20"/>
-      <c r="U8" s="22"/>
-      <c r="V8" s="23" t="s">
-        <v>20</v>
+      <c r="U8" s="21"/>
+      <c r="V8" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="W8" s="20"/>
       <c r="X8" s="20"/>
-      <c r="Y8" s="22"/>
-      <c r="Z8" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" s="22"/>
-      <c r="AB8" s="29" t="s">
-        <v>16</v>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="25" t="s">
+        <v>14</v>
       </c>
       <c r="AC8" s="20"/>
       <c r="AD8" s="20"/>
-      <c r="AE8" s="22"/>
-      <c r="AF8" s="31" t="s">
-        <v>17</v>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="27" t="s">
+        <v>15</v>
       </c>
       <c r="AG8" s="20"/>
       <c r="AH8" s="20"/>
-      <c r="AI8" s="22"/>
-      <c r="AJ8" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK8" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL8" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="AM8" s="22"/>
-      <c r="AN8" s="31" t="s">
+      <c r="AI8" s="21"/>
+      <c r="AJ8" s="29" t="s">
         <v>16</v>
+      </c>
+      <c r="AK8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL8" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM8" s="21"/>
+      <c r="AN8" s="27" t="s">
+        <v>14</v>
       </c>
       <c r="AO8" s="20"/>
       <c r="AP8" s="20"/>
-      <c r="AQ8" s="22"/>
-      <c r="AR8" s="34" t="s">
-        <v>17</v>
+      <c r="AQ8" s="21"/>
+      <c r="AR8" s="33" t="s">
+        <v>15</v>
       </c>
       <c r="AS8" s="20"/>
       <c r="AT8" s="20"/>
-      <c r="AU8" s="22"/>
-      <c r="AV8" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="AW8" s="32" t="s">
-        <v>19</v>
+      <c r="AU8" s="21"/>
+      <c r="AV8" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AW8" s="29" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
       <c r="E9" s="37"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
       <c r="I9" s="37"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
       <c r="M9" s="37"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
       <c r="Q9" s="37"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="36"/>
-      <c r="T9" s="36"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
       <c r="U9" s="37"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="36"/>
-      <c r="X9" s="36"/>
+      <c r="V9" s="34"/>
+      <c r="W9" s="35"/>
+      <c r="X9" s="35"/>
       <c r="Y9" s="37"/>
-      <c r="Z9" s="35"/>
+      <c r="Z9" s="34"/>
       <c r="AA9" s="37"/>
-      <c r="AB9" s="35"/>
-      <c r="AC9" s="36"/>
-      <c r="AD9" s="36"/>
+      <c r="AB9" s="34"/>
+      <c r="AC9" s="35"/>
+      <c r="AD9" s="35"/>
       <c r="AE9" s="37"/>
-      <c r="AF9" s="35"/>
-      <c r="AG9" s="36"/>
-      <c r="AH9" s="36"/>
+      <c r="AF9" s="34"/>
+      <c r="AG9" s="35"/>
+      <c r="AH9" s="35"/>
       <c r="AI9" s="37"/>
       <c r="AJ9" s="38"/>
       <c r="AK9" s="38"/>
-      <c r="AL9" s="35"/>
+      <c r="AL9" s="34"/>
       <c r="AM9" s="37"/>
-      <c r="AN9" s="35"/>
-      <c r="AO9" s="36"/>
-      <c r="AP9" s="36"/>
+      <c r="AN9" s="34"/>
+      <c r="AO9" s="35"/>
+      <c r="AP9" s="35"/>
       <c r="AQ9" s="37"/>
-      <c r="AR9" s="35"/>
-      <c r="AS9" s="36"/>
-      <c r="AT9" s="36"/>
+      <c r="AR9" s="34"/>
+      <c r="AS9" s="35"/>
+      <c r="AT9" s="35"/>
       <c r="AU9" s="37"/>
       <c r="AV9" s="38"/>
       <c r="AW9" s="38"/>
     </row>
     <row r="10">
       <c r="A10" s="39" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B10" s="40">
         <v>1.0</v>
@@ -2839,64 +3059,64 @@
       <c r="AE10" s="43">
         <v>4.0</v>
       </c>
-      <c r="AF10" s="33">
+      <c r="AF10" s="31">
         <v>1.0</v>
       </c>
-      <c r="AG10" s="33">
+      <c r="AG10" s="31">
         <v>2.0</v>
       </c>
-      <c r="AH10" s="33">
+      <c r="AH10" s="31">
         <v>3.0</v>
       </c>
-      <c r="AI10" s="33">
+      <c r="AI10" s="31">
         <v>4.0</v>
       </c>
-      <c r="AJ10" s="32">
+      <c r="AJ10" s="29">
         <v>1.0</v>
       </c>
-      <c r="AK10" s="33">
+      <c r="AK10" s="31">
         <v>1.0</v>
       </c>
-      <c r="AL10" s="32">
+      <c r="AL10" s="29">
         <v>1.0</v>
       </c>
-      <c r="AM10" s="32">
+      <c r="AM10" s="29">
         <v>2.0</v>
       </c>
-      <c r="AN10" s="33">
+      <c r="AN10" s="31">
         <v>1.0</v>
       </c>
-      <c r="AO10" s="33">
+      <c r="AO10" s="31">
         <v>2.0</v>
       </c>
-      <c r="AP10" s="33">
+      <c r="AP10" s="31">
         <v>3.0</v>
       </c>
-      <c r="AQ10" s="33">
+      <c r="AQ10" s="31">
         <v>4.0</v>
       </c>
-      <c r="AR10" s="32">
+      <c r="AR10" s="29">
         <v>1.0</v>
       </c>
-      <c r="AS10" s="32">
+      <c r="AS10" s="29">
         <v>2.0</v>
       </c>
-      <c r="AT10" s="32">
+      <c r="AT10" s="29">
         <v>3.0</v>
       </c>
-      <c r="AU10" s="32">
+      <c r="AU10" s="29">
         <v>4.0</v>
       </c>
-      <c r="AV10" s="33">
+      <c r="AV10" s="31">
         <v>1.0</v>
       </c>
-      <c r="AW10" s="32">
+      <c r="AW10" s="29">
         <v>1.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="44" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
@@ -2952,148 +3172,148 @@
         <v>1.0</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D12" s="46" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F12" s="47" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G12" s="47" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H12" s="47" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I12" s="47" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J12" s="46" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K12" s="46" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="L12" s="46" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M12" s="46" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="N12" s="47" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="O12" s="47" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P12" s="47" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="Q12" s="47" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="R12" s="46" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="S12" s="46" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="T12" s="46" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="U12" s="46" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="V12" s="47" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="W12" s="47" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="X12" s="47" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="Y12" s="47" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="Z12" s="46" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AA12" s="46" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AB12" s="47" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="AC12" s="47" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AD12" s="47" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AE12" s="47" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AF12" s="46" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AG12" s="46" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AH12" s="46" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="AI12" s="46" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="AJ12" s="47" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AK12" s="46" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="AL12" s="47" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AM12" s="47" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AN12" s="46" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AO12" s="46" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AP12" s="46" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AQ12" s="46" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AR12" s="47" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="AS12" s="47" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AT12" s="47" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AU12" s="47" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AV12" s="46" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AW12" s="47" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13">
@@ -3101,148 +3321,148 @@
         <v>2.0</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D13" s="46" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F13" s="47" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G13" s="47" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H13" s="47" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="I13" s="47" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="J13" s="46" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K13" s="46" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="L13" s="46" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M13" s="46" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="N13" s="47" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="O13" s="47" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="P13" s="47" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q13" s="47" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="R13" s="46" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="S13" s="46" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="T13" s="46" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="U13" s="46" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="V13" s="47" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="W13" s="47" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="X13" s="47" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="Y13" s="47" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="Z13" s="46" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="AA13" s="46" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="AB13" s="47" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="AC13" s="47" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="AD13" s="47" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="AE13" s="47" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AF13" s="46" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="AG13" s="46" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="AH13" s="46" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="AI13" s="46" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="AJ13" s="47" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="AK13" s="46" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AL13" s="47" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AM13" s="47" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AN13" s="46" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="AO13" s="46" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AP13" s="46" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AQ13" s="46" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AR13" s="47" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AS13" s="47" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AT13" s="47" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AU13" s="47" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AV13" s="46" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AW13" s="47" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14">
@@ -3250,148 +3470,148 @@
         <v>3.0</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D14" s="46" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F14" s="47" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G14" s="47" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H14" s="47" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="I14" s="47" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="J14" s="46" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="K14" s="46" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="L14" s="46" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="M14" s="46" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="N14" s="47" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="O14" s="47" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="P14" s="47" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="Q14" s="47" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="R14" s="46" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="S14" s="46" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="T14" s="46" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="U14" s="46" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="V14" s="47" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="W14" s="47" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="X14" s="47" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="Y14" s="47" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="Z14" s="46" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AA14" s="46" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AB14" s="47" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AC14" s="47" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AD14" s="47" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AE14" s="47" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AF14" s="46" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AG14" s="46" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="AH14" s="46" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="AI14" s="46" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="AJ14" s="47" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AK14" s="46" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AL14" s="47" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AM14" s="47" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="AN14" s="46" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="AO14" s="46" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AP14" s="46" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="AQ14" s="46" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="AR14" s="47" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="AS14" s="47" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="AT14" s="47" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="AU14" s="47" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="AV14" s="46" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AW14" s="47" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15">
@@ -3399,448 +3619,449 @@
         <v>4.0</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D15" s="46" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F15" s="47" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="G15" s="47" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H15" s="47" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="I15" s="47" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="J15" s="46" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="K15" s="46" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="L15" s="46" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="M15" s="46" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="N15" s="47" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="O15" s="47" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="P15" s="47" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="Q15" s="47" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="R15" s="46" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="S15" s="46" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="T15" s="46" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U15" s="46" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="V15" s="47" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="W15" s="47" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="X15" s="47" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="Y15" s="47" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="Z15" s="46" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="AA15" s="46" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="AB15" s="47" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="AC15" s="47" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AD15" s="47" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="AE15" s="47" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AF15" s="46" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="AG15" s="46" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="AH15" s="46" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AI15" s="46" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="AJ15" s="47" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="AK15" s="46" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="AL15" s="47" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AM15" s="47" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AN15" s="46" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="AO15" s="46" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="AP15" s="46" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="AQ15" s="46" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="AR15" s="47" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="AS15" s="47" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="AT15" s="47" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="AU15" s="47" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="AV15" s="46" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="AW15" s="47" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="48">
+      <c r="A16" s="45">
         <v>5.0</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="50"/>
-      <c r="P16" s="50"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="49"/>
-      <c r="S16" s="49"/>
-      <c r="T16" s="49"/>
-      <c r="U16" s="49"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="50"/>
-      <c r="X16" s="50"/>
-      <c r="Y16" s="50"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="48"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="48"/>
+      <c r="U16" s="48"/>
+      <c r="V16" s="49"/>
+      <c r="W16" s="49"/>
+      <c r="X16" s="49"/>
+      <c r="Y16" s="49"/>
       <c r="Z16" s="46" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="AA16" s="46" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="AB16" s="47" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="AC16" s="47" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="AD16" s="47" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="AE16" s="47" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="AF16" s="46" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="AG16" s="46" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="AH16" s="46" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="AI16" s="46" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="AJ16" s="47" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="AK16" s="46" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="AL16" s="47" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="AM16" s="47" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="AN16" s="46" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="AO16" s="46" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="AP16" s="46" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="AQ16" s="46" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="AR16" s="47" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="AS16" s="47" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="AT16" s="47" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="AU16" s="47" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="AV16" s="46" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="AW16" s="47" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="B17" s="51">
+        <v>245</v>
+      </c>
+      <c r="B17" s="50">
         <f t="shared" ref="B17:AW17" si="1">SUM(B12:B15)</f>
         <v>0</v>
       </c>
-      <c r="C17" s="51">
+      <c r="C17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D17" s="51">
+      <c r="D17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E17" s="51">
+      <c r="E17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F17" s="51">
+      <c r="F17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G17" s="51">
+      <c r="G17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H17" s="51">
+      <c r="H17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I17" s="51">
+      <c r="I17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J17" s="51">
+      <c r="J17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K17" s="51">
+      <c r="K17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L17" s="51">
+      <c r="L17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M17" s="51">
+      <c r="M17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N17" s="51">
+      <c r="N17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O17" s="51">
+      <c r="O17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P17" s="51">
+      <c r="P17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="51">
+      <c r="Q17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R17" s="51">
+      <c r="R17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S17" s="51">
+      <c r="S17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T17" s="51">
+      <c r="T17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U17" s="51">
+      <c r="U17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V17" s="51">
+      <c r="V17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W17" s="51">
+      <c r="W17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X17" s="51">
+      <c r="X17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y17" s="51">
+      <c r="Y17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z17" s="51">
+      <c r="Z17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA17" s="51">
+      <c r="AA17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB17" s="51">
+      <c r="AB17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC17" s="51">
+      <c r="AC17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AD17" s="51">
+      <c r="AD17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE17" s="51">
+      <c r="AE17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AF17" s="51">
+      <c r="AF17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AG17" s="51">
+      <c r="AG17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AH17" s="51">
+      <c r="AH17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AI17" s="51">
+      <c r="AI17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ17" s="51">
+      <c r="AJ17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AK17" s="51">
+      <c r="AK17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AL17" s="51">
+      <c r="AL17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AM17" s="51">
+      <c r="AM17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AN17" s="51">
+      <c r="AN17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AO17" s="51">
+      <c r="AO17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AP17" s="51">
+      <c r="AP17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AQ17" s="51">
+      <c r="AQ17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AR17" s="51">
+      <c r="AR17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AS17" s="51">
+      <c r="AS17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AT17" s="51">
+      <c r="AT17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AU17" s="51">
+      <c r="AU17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AV17" s="51">
+      <c r="AV17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AW17" s="51">
+      <c r="AW17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
+    <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -4820,78 +5041,77 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="Z7:AK7"/>
+    <mergeCell ref="AF8:AI9"/>
+    <mergeCell ref="AD10:AD11"/>
+    <mergeCell ref="AF10:AF11"/>
+    <mergeCell ref="X10:X11"/>
+    <mergeCell ref="AW8:AW9"/>
+    <mergeCell ref="AR8:AU9"/>
+    <mergeCell ref="AL7:AW7"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="AP10:AP11"/>
     <mergeCell ref="AL10:AL11"/>
-    <mergeCell ref="AE10:AE11"/>
-    <mergeCell ref="AF10:AF11"/>
     <mergeCell ref="AG10:AG11"/>
-    <mergeCell ref="AH10:AH11"/>
-    <mergeCell ref="AJ10:AJ11"/>
-    <mergeCell ref="AK10:AK11"/>
-    <mergeCell ref="AI10:AI11"/>
-    <mergeCell ref="AA10:AA11"/>
-    <mergeCell ref="AB10:AB11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="AN8:AQ9"/>
+    <mergeCell ref="AL8:AM9"/>
+    <mergeCell ref="AV8:AV9"/>
+    <mergeCell ref="AV10:AV11"/>
+    <mergeCell ref="AW10:AW11"/>
+    <mergeCell ref="AU10:AU11"/>
     <mergeCell ref="AN10:AN11"/>
     <mergeCell ref="AO10:AO11"/>
     <mergeCell ref="AQ10:AQ11"/>
     <mergeCell ref="AR10:AR11"/>
     <mergeCell ref="AS10:AS11"/>
     <mergeCell ref="AT10:AT11"/>
-    <mergeCell ref="AP10:AP11"/>
+    <mergeCell ref="AM10:AM11"/>
+    <mergeCell ref="AJ10:AJ11"/>
+    <mergeCell ref="F8:I9"/>
+    <mergeCell ref="J8:M9"/>
+    <mergeCell ref="V8:Y9"/>
+    <mergeCell ref="AB8:AE9"/>
+    <mergeCell ref="Z8:AA9"/>
+    <mergeCell ref="B7:Y7"/>
+    <mergeCell ref="R8:U9"/>
+    <mergeCell ref="N8:Q9"/>
+    <mergeCell ref="A6:AW6"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="AH10:AH11"/>
+    <mergeCell ref="AK10:AK11"/>
+    <mergeCell ref="AI10:AI11"/>
+    <mergeCell ref="AB10:AB11"/>
+    <mergeCell ref="AC10:AC11"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="V10:V11"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="T10:T11"/>
     <mergeCell ref="S10:S11"/>
-    <mergeCell ref="AM10:AM11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="X10:X11"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="W10:W11"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="AA10:AA11"/>
+    <mergeCell ref="AE10:AE11"/>
+    <mergeCell ref="B8:E9"/>
+    <mergeCell ref="A7:A9"/>
     <mergeCell ref="AJ8:AJ9"/>
     <mergeCell ref="AK8:AK9"/>
-    <mergeCell ref="F8:I9"/>
-    <mergeCell ref="B8:E9"/>
-    <mergeCell ref="R8:U9"/>
-    <mergeCell ref="V8:Y9"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="J8:M9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:Y7"/>
-    <mergeCell ref="A6:AW6"/>
-    <mergeCell ref="AL8:AM9"/>
-    <mergeCell ref="AB8:AE9"/>
-    <mergeCell ref="Z8:AA9"/>
-    <mergeCell ref="AF8:AI9"/>
-    <mergeCell ref="AC10:AC11"/>
-    <mergeCell ref="AD10:AD11"/>
-    <mergeCell ref="AL7:AW7"/>
-    <mergeCell ref="Z7:AK7"/>
-    <mergeCell ref="AV10:AV11"/>
-    <mergeCell ref="AU10:AU11"/>
-    <mergeCell ref="AV8:AV9"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="P10:P11"/>
-    <mergeCell ref="N8:Q9"/>
-    <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="V10:V11"/>
-    <mergeCell ref="W10:W11"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="AW8:AW9"/>
-    <mergeCell ref="AW10:AW11"/>
-    <mergeCell ref="AN8:AQ9"/>
-    <mergeCell ref="AR8:AU9"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>